<commit_message>
Update on 20200717 part 2
</commit_message>
<xml_diff>
--- a/文档/测试工作相关/End-to-end integration test/测试内容相关/2020/20200716/叠加网光网用户(206440738 )/叠加网光网用户(206440738 )测试报告.xlsx
+++ b/文档/测试工作相关/End-to-end integration test/测试内容相关/2020/20200716/叠加网光网用户(206440738 )/叠加网光网用户(206440738 )测试报告.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>测试状态</t>
   </si>
@@ -235,14 +235,6 @@
   </si>
   <si>
     <t>处理中</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>有线宽带割接（onu逻辑号变化）</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>有线宽带割接（onu逻辑号无变化）</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -396,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -468,16 +460,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -783,7 +766,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IT6"/>
+  <dimension ref="A1:IT4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -818,19 +801,19 @@
       <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H1" s="8" t="s">
@@ -1114,52 +1097,52 @@
       <c r="B2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="24"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="15"/>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="33">
-        <v>5</v>
-      </c>
-      <c r="I2" s="29" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="30">
+        <v>3</v>
+      </c>
+      <c r="I2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="34">
+      <c r="L2" s="31">
         <v>206440738</v>
       </c>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="N2" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="29">
+      <c r="P2" s="26">
         <v>206442027</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="Q2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="29">
+      <c r="R2" s="26">
         <v>20200728</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="S2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="29"/>
+      <c r="T2" s="26"/>
       <c r="U2" s="23"/>
       <c r="V2" s="23"/>
       <c r="W2" s="23"/>
@@ -1402,26 +1385,26 @@
       <c r="B3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="24"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
       <c r="U3" s="23"/>
       <c r="V3" s="23"/>
       <c r="W3" s="23"/>
@@ -1664,26 +1647,26 @@
       <c r="B4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="28"/>
+      <c r="C4" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="25"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
       <c r="U4" s="23"/>
       <c r="V4" s="23"/>
       <c r="W4" s="23"/>
@@ -1919,313 +1902,23 @@
       <c r="IS4" s="23"/>
       <c r="IT4" s="23"/>
     </row>
-    <row r="5" spans="1:254" ht="24">
-      <c r="A5" s="20">
-        <v>4</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
-      <c r="AD5" s="23"/>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="23"/>
-      <c r="AG5" s="23"/>
-      <c r="AH5" s="23"/>
-      <c r="AI5" s="23"/>
-      <c r="AJ5" s="23"/>
-      <c r="AK5" s="23"/>
-      <c r="AL5" s="23"/>
-      <c r="AM5" s="23"/>
-      <c r="AN5" s="23"/>
-      <c r="AO5" s="23"/>
-      <c r="AP5" s="23"/>
-      <c r="AQ5" s="23"/>
-      <c r="AR5" s="23"/>
-      <c r="AS5" s="23"/>
-      <c r="AT5" s="23"/>
-      <c r="AU5" s="23"/>
-      <c r="AV5" s="23"/>
-      <c r="AW5" s="23"/>
-      <c r="AX5" s="23"/>
-      <c r="AY5" s="23"/>
-      <c r="AZ5" s="23"/>
-      <c r="BA5" s="23"/>
-      <c r="BB5" s="23"/>
-      <c r="BC5" s="23"/>
-      <c r="BD5" s="23"/>
-      <c r="BE5" s="23"/>
-      <c r="BF5" s="23"/>
-      <c r="BG5" s="23"/>
-      <c r="BH5" s="23"/>
-      <c r="BI5" s="23"/>
-      <c r="BJ5" s="23"/>
-      <c r="BK5" s="23"/>
-      <c r="BL5" s="23"/>
-      <c r="BM5" s="23"/>
-      <c r="BN5" s="23"/>
-      <c r="BO5" s="23"/>
-      <c r="BP5" s="23"/>
-      <c r="BQ5" s="23"/>
-      <c r="BR5" s="23"/>
-      <c r="BS5" s="23"/>
-      <c r="BT5" s="23"/>
-      <c r="BU5" s="23"/>
-      <c r="BV5" s="23"/>
-      <c r="BW5" s="23"/>
-      <c r="BX5" s="23"/>
-      <c r="BY5" s="23"/>
-      <c r="BZ5" s="23"/>
-      <c r="CA5" s="23"/>
-      <c r="CB5" s="23"/>
-      <c r="CC5" s="23"/>
-      <c r="CD5" s="23"/>
-      <c r="CE5" s="23"/>
-      <c r="CF5" s="23"/>
-      <c r="CG5" s="23"/>
-      <c r="CH5" s="23"/>
-      <c r="CI5" s="23"/>
-      <c r="CJ5" s="23"/>
-      <c r="CK5" s="23"/>
-      <c r="CL5" s="23"/>
-      <c r="CM5" s="23"/>
-      <c r="CN5" s="23"/>
-      <c r="CO5" s="23"/>
-      <c r="CP5" s="23"/>
-      <c r="CQ5" s="23"/>
-      <c r="CR5" s="23"/>
-      <c r="CS5" s="23"/>
-      <c r="CT5" s="23"/>
-      <c r="CU5" s="23"/>
-      <c r="CV5" s="23"/>
-      <c r="CW5" s="23"/>
-      <c r="CX5" s="23"/>
-      <c r="CY5" s="23"/>
-      <c r="CZ5" s="23"/>
-      <c r="DA5" s="23"/>
-      <c r="DB5" s="23"/>
-      <c r="DC5" s="23"/>
-      <c r="DD5" s="23"/>
-      <c r="DE5" s="23"/>
-      <c r="DF5" s="23"/>
-      <c r="DG5" s="23"/>
-      <c r="DH5" s="23"/>
-      <c r="DI5" s="23"/>
-      <c r="DJ5" s="23"/>
-      <c r="DK5" s="23"/>
-      <c r="DL5" s="23"/>
-      <c r="DM5" s="23"/>
-      <c r="DN5" s="23"/>
-      <c r="DO5" s="23"/>
-      <c r="DP5" s="23"/>
-      <c r="DQ5" s="23"/>
-      <c r="DR5" s="23"/>
-      <c r="DS5" s="23"/>
-      <c r="DT5" s="23"/>
-      <c r="DU5" s="23"/>
-      <c r="DV5" s="23"/>
-      <c r="DW5" s="23"/>
-      <c r="DX5" s="23"/>
-      <c r="DY5" s="23"/>
-      <c r="DZ5" s="23"/>
-      <c r="EA5" s="23"/>
-      <c r="EB5" s="23"/>
-      <c r="EC5" s="23"/>
-      <c r="ED5" s="23"/>
-      <c r="EE5" s="23"/>
-      <c r="EF5" s="23"/>
-      <c r="EG5" s="23"/>
-      <c r="EH5" s="23"/>
-      <c r="EI5" s="23"/>
-      <c r="EJ5" s="23"/>
-      <c r="EK5" s="23"/>
-      <c r="EL5" s="23"/>
-      <c r="EM5" s="23"/>
-      <c r="EN5" s="23"/>
-      <c r="EO5" s="23"/>
-      <c r="EP5" s="23"/>
-      <c r="EQ5" s="23"/>
-      <c r="ER5" s="23"/>
-      <c r="ES5" s="23"/>
-      <c r="ET5" s="23"/>
-      <c r="EU5" s="23"/>
-      <c r="EV5" s="23"/>
-      <c r="EW5" s="23"/>
-      <c r="EX5" s="23"/>
-      <c r="EY5" s="23"/>
-      <c r="EZ5" s="23"/>
-      <c r="FA5" s="23"/>
-      <c r="FB5" s="23"/>
-      <c r="FC5" s="23"/>
-      <c r="FD5" s="23"/>
-      <c r="FE5" s="23"/>
-      <c r="FF5" s="23"/>
-      <c r="FG5" s="23"/>
-      <c r="FH5" s="23"/>
-      <c r="FI5" s="23"/>
-      <c r="FJ5" s="23"/>
-      <c r="FK5" s="23"/>
-      <c r="FL5" s="23"/>
-      <c r="FM5" s="23"/>
-      <c r="FN5" s="23"/>
-      <c r="FO5" s="23"/>
-      <c r="FP5" s="23"/>
-      <c r="FQ5" s="23"/>
-      <c r="FR5" s="23"/>
-      <c r="FS5" s="23"/>
-      <c r="FT5" s="23"/>
-      <c r="FU5" s="23"/>
-      <c r="FV5" s="23"/>
-      <c r="FW5" s="23"/>
-      <c r="FX5" s="23"/>
-      <c r="FY5" s="23"/>
-      <c r="FZ5" s="23"/>
-      <c r="GA5" s="23"/>
-      <c r="GB5" s="23"/>
-      <c r="GC5" s="23"/>
-      <c r="GD5" s="23"/>
-      <c r="GE5" s="23"/>
-      <c r="GF5" s="23"/>
-      <c r="GG5" s="23"/>
-      <c r="GH5" s="23"/>
-      <c r="GI5" s="23"/>
-      <c r="GJ5" s="23"/>
-      <c r="GK5" s="23"/>
-      <c r="GL5" s="23"/>
-      <c r="GM5" s="23"/>
-      <c r="GN5" s="23"/>
-      <c r="GO5" s="23"/>
-      <c r="GP5" s="23"/>
-      <c r="GQ5" s="23"/>
-      <c r="GR5" s="23"/>
-      <c r="GS5" s="23"/>
-      <c r="GT5" s="23"/>
-      <c r="GU5" s="23"/>
-      <c r="GV5" s="23"/>
-      <c r="GW5" s="23"/>
-      <c r="GX5" s="23"/>
-      <c r="GY5" s="23"/>
-      <c r="GZ5" s="23"/>
-      <c r="HA5" s="23"/>
-      <c r="HB5" s="23"/>
-      <c r="HC5" s="23"/>
-      <c r="HD5" s="23"/>
-      <c r="HE5" s="23"/>
-      <c r="HF5" s="23"/>
-      <c r="HG5" s="23"/>
-      <c r="HH5" s="23"/>
-      <c r="HI5" s="23"/>
-      <c r="HJ5" s="23"/>
-      <c r="HK5" s="23"/>
-      <c r="HL5" s="23"/>
-      <c r="HM5" s="23"/>
-      <c r="HN5" s="23"/>
-      <c r="HO5" s="23"/>
-      <c r="HP5" s="23"/>
-      <c r="HQ5" s="23"/>
-      <c r="HR5" s="23"/>
-      <c r="HS5" s="23"/>
-      <c r="HT5" s="23"/>
-      <c r="HU5" s="23"/>
-      <c r="HV5" s="23"/>
-      <c r="HW5" s="23"/>
-      <c r="HX5" s="23"/>
-      <c r="HY5" s="23"/>
-      <c r="HZ5" s="23"/>
-      <c r="IA5" s="23"/>
-      <c r="IB5" s="23"/>
-      <c r="IC5" s="23"/>
-      <c r="ID5" s="23"/>
-      <c r="IE5" s="23"/>
-      <c r="IF5" s="23"/>
-      <c r="IG5" s="23"/>
-      <c r="IH5" s="23"/>
-      <c r="II5" s="23"/>
-      <c r="IJ5" s="23"/>
-      <c r="IK5" s="23"/>
-      <c r="IL5" s="23"/>
-      <c r="IM5" s="23"/>
-      <c r="IN5" s="23"/>
-      <c r="IO5" s="23"/>
-      <c r="IP5" s="23"/>
-      <c r="IQ5" s="23"/>
-      <c r="IR5" s="23"/>
-      <c r="IS5" s="23"/>
-      <c r="IT5" s="23"/>
-    </row>
-    <row r="6" spans="1:254" ht="24">
-      <c r="A6" s="20">
-        <v>5</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="Q2:Q6"/>
-    <mergeCell ref="R2:R6"/>
-    <mergeCell ref="S2:S6"/>
-    <mergeCell ref="T2:T6"/>
-    <mergeCell ref="F2:F6"/>
-    <mergeCell ref="H2:H6"/>
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="K2:K6"/>
-    <mergeCell ref="L2:L6"/>
-    <mergeCell ref="M2:M6"/>
-    <mergeCell ref="N2:N6"/>
-    <mergeCell ref="O2:O6"/>
-    <mergeCell ref="P2:P6"/>
-    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="R2:R4"/>
+    <mergeCell ref="S2:S4"/>
+    <mergeCell ref="T2:T4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="G2:G4"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2299,7 +1992,7 @@
         <v>44029.451388888891</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>41</v>

</xml_diff>